<commit_message>
more work on multi-bit
</commit_message>
<xml_diff>
--- a/densities.xlsx
+++ b/densities.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\.spyder-py3\Robert_Python\Steganography\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03366EB-DF8C-4E28-8DC4-C0FB331745D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD560256-8233-4079-9E2C-2CDE24137270}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -426,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AR98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="F92" sqref="F92"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4492,7 +4492,7 @@
         <v>3</v>
       </c>
       <c r="D30">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E30">
         <v>7</v>
@@ -4770,19 +4770,19 @@
     </row>
     <row r="32" spans="1:44" x14ac:dyDescent="0.3">
       <c r="B32">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C32">
         <f>POWER(2,B32)</f>
-        <v>8388608</v>
+        <v>2097152</v>
       </c>
       <c r="D32">
         <f>_xlfn.CEILING.MATH(C32/(C30*D30))</f>
-        <v>1398102</v>
+        <v>699051</v>
       </c>
       <c r="E32">
         <f>_xlfn.CEILING.MATH(SQRT(D32))</f>
-        <v>1183</v>
+        <v>837</v>
       </c>
       <c r="M32">
         <f t="shared" ref="M32:AR32" si="27">LOG(M10,2)</f>
@@ -5189,7 +5189,7 @@
       </c>
       <c r="D35">
         <f>_xlfn.FLOOR.MATH(LOG(COMBIN($C$32,C35),2))</f>
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E35">
         <f>_xlfn.FLOOR.MATH(D35/$E$30)</f>
@@ -5331,11 +5331,11 @@
       </c>
       <c r="D36">
         <f t="shared" ref="D36:D65" si="31">_xlfn.FLOOR.MATH(LOG(COMBIN($C$32,C36),2))</f>
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E36">
         <f t="shared" ref="E36:E98" si="32">_xlfn.FLOOR.MATH(D36/$E$30)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="M36">
         <f t="shared" ref="M36:AR36" si="33">LOG(M14,2)</f>
@@ -5473,11 +5473,11 @@
       </c>
       <c r="D37">
         <f t="shared" si="31"/>
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E37">
         <f t="shared" si="32"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M37">
         <f t="shared" ref="M37:AR37" si="35">LOG(M15,2)</f>
@@ -5615,11 +5615,11 @@
       </c>
       <c r="D38">
         <f t="shared" si="31"/>
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="E38">
         <f t="shared" si="32"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="M38">
         <f t="shared" ref="M38:AR38" si="36">LOG(M16,2)</f>
@@ -5757,11 +5757,11 @@
       </c>
       <c r="D39">
         <f t="shared" si="31"/>
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="E39">
         <f t="shared" si="32"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M39">
         <f t="shared" ref="M39:AR39" si="37">LOG(M17,2)</f>
@@ -5899,11 +5899,11 @@
       </c>
       <c r="D40">
         <f t="shared" si="31"/>
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="E40">
         <f t="shared" si="32"/>
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="M40">
         <f t="shared" ref="M40:AR40" si="38">LOG(M18,2)</f>
@@ -6041,11 +6041,11 @@
       </c>
       <c r="D41">
         <f t="shared" si="31"/>
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="E41">
         <f t="shared" si="32"/>
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M41">
         <f t="shared" ref="M41:AR41" si="39">LOG(M19,2)</f>
@@ -6183,11 +6183,11 @@
       </c>
       <c r="D42">
         <f t="shared" si="31"/>
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="E42">
         <f t="shared" si="32"/>
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="M42">
         <f t="shared" ref="M42:AR42" si="40">LOG(M20,2)</f>
@@ -6325,11 +6325,11 @@
       </c>
       <c r="D43">
         <f t="shared" si="31"/>
-        <v>188</v>
+        <v>170</v>
       </c>
       <c r="E43">
         <f t="shared" si="32"/>
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M43">
         <f t="shared" ref="M43:AR43" si="41">LOG(M21,2)</f>
@@ -6467,11 +6467,11 @@
       </c>
       <c r="D44">
         <f t="shared" si="31"/>
-        <v>208</v>
+        <v>188</v>
       </c>
       <c r="E44">
         <f t="shared" si="32"/>
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="M44">
         <f t="shared" ref="M44:AR44" si="42">LOG(M22,2)</f>
@@ -6609,11 +6609,11 @@
       </c>
       <c r="D45">
         <f t="shared" si="31"/>
-        <v>227</v>
+        <v>205</v>
       </c>
       <c r="E45">
         <f t="shared" si="32"/>
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="M45">
         <f t="shared" ref="M45:AR45" si="43">LOG(M23,2)</f>
@@ -6751,11 +6751,11 @@
       </c>
       <c r="D46">
         <f t="shared" si="31"/>
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="E46">
         <f t="shared" si="32"/>
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="2:44" x14ac:dyDescent="0.3">
@@ -6765,11 +6765,11 @@
       </c>
       <c r="D47">
         <f t="shared" si="31"/>
-        <v>266</v>
+        <v>240</v>
       </c>
       <c r="E47">
         <f t="shared" si="32"/>
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="M47" t="s">
         <v>15</v>
@@ -6782,11 +6782,11 @@
       </c>
       <c r="D48">
         <f t="shared" si="31"/>
-        <v>285</v>
+        <v>257</v>
       </c>
       <c r="E48">
         <f t="shared" si="32"/>
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="M48">
         <f>M26/M$3</f>
@@ -6924,11 +6924,11 @@
       </c>
       <c r="D49">
         <f t="shared" si="31"/>
-        <v>304</v>
+        <v>274</v>
       </c>
       <c r="E49">
         <f t="shared" si="32"/>
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="M49">
         <f t="shared" ref="M49:AR49" si="45">M27/M$3</f>
@@ -7066,11 +7066,11 @@
       </c>
       <c r="D50">
         <f t="shared" si="31"/>
-        <v>323</v>
+        <v>291</v>
       </c>
       <c r="E50">
         <f t="shared" si="32"/>
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="M50">
         <f t="shared" ref="M50:AR50" si="46">M28/M$3</f>
@@ -7208,11 +7208,11 @@
       </c>
       <c r="D51">
         <f t="shared" si="31"/>
-        <v>342</v>
+        <v>308</v>
       </c>
       <c r="E51">
         <f t="shared" si="32"/>
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="M51">
         <f t="shared" ref="M51:AR51" si="47">M29/M$3</f>
@@ -7350,11 +7350,11 @@
       </c>
       <c r="D52">
         <f t="shared" si="31"/>
-        <v>361</v>
+        <v>325</v>
       </c>
       <c r="E52">
         <f t="shared" si="32"/>
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="M52">
         <f t="shared" ref="M52:AR52" si="48">M30/M$3</f>
@@ -7492,11 +7492,11 @@
       </c>
       <c r="D53">
         <f t="shared" si="31"/>
-        <v>380</v>
+        <v>342</v>
       </c>
       <c r="E53">
         <f t="shared" si="32"/>
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="M53">
         <f t="shared" ref="M53:AR53" si="49">M31/M$3</f>
@@ -7634,11 +7634,11 @@
       </c>
       <c r="D54">
         <f t="shared" si="31"/>
-        <v>398</v>
+        <v>358</v>
       </c>
       <c r="E54">
         <f t="shared" si="32"/>
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="M54">
         <f t="shared" ref="M54:AR54" si="50">M32/M$3</f>
@@ -7776,11 +7776,11 @@
       </c>
       <c r="D55">
         <f t="shared" si="31"/>
-        <v>417</v>
+        <v>375</v>
       </c>
       <c r="E55">
         <f t="shared" si="32"/>
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="M55">
         <f t="shared" ref="M55:AR55" si="51">M33/M$3</f>
@@ -7918,11 +7918,11 @@
       </c>
       <c r="D56">
         <f t="shared" si="31"/>
-        <v>436</v>
+        <v>392</v>
       </c>
       <c r="E56">
         <f t="shared" si="32"/>
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="M56">
         <f t="shared" ref="M56:AR56" si="52">M34/M$3</f>
@@ -8060,11 +8060,11 @@
       </c>
       <c r="D57">
         <f t="shared" si="31"/>
-        <v>454</v>
+        <v>408</v>
       </c>
       <c r="E57">
         <f t="shared" si="32"/>
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="M57">
         <f t="shared" ref="M57:AR57" si="53">M35/M$3</f>
@@ -8202,11 +8202,11 @@
       </c>
       <c r="D58">
         <f t="shared" si="31"/>
-        <v>472</v>
+        <v>424</v>
       </c>
       <c r="E58">
         <f t="shared" si="32"/>
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="M58">
         <f t="shared" ref="M58:AR58" si="54">M36/M$3</f>
@@ -8344,11 +8344,11 @@
       </c>
       <c r="D59">
         <f t="shared" si="31"/>
-        <v>491</v>
+        <v>441</v>
       </c>
       <c r="E59">
         <f t="shared" si="32"/>
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="M59">
         <f t="shared" ref="M59:AR59" si="55">M37/M$3</f>
@@ -8486,11 +8486,11 @@
       </c>
       <c r="D60">
         <f t="shared" si="31"/>
-        <v>509</v>
+        <v>457</v>
       </c>
       <c r="E60">
         <f t="shared" si="32"/>
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="M60">
         <f t="shared" ref="M60:AR60" si="56">M38/M$3</f>
@@ -8628,11 +8628,11 @@
       </c>
       <c r="D61">
         <f t="shared" si="31"/>
-        <v>527</v>
+        <v>473</v>
       </c>
       <c r="E61">
         <f t="shared" si="32"/>
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="M61">
         <f t="shared" ref="M61:AR61" si="57">M39/M$3</f>
@@ -8770,11 +8770,11 @@
       </c>
       <c r="D62">
         <f t="shared" si="31"/>
-        <v>546</v>
+        <v>490</v>
       </c>
       <c r="E62">
         <f t="shared" si="32"/>
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="M62">
         <f t="shared" ref="M62:AR62" si="58">M40/M$3</f>
@@ -8912,11 +8912,11 @@
       </c>
       <c r="D63">
         <f t="shared" si="31"/>
-        <v>564</v>
+        <v>506</v>
       </c>
       <c r="E63">
         <f t="shared" si="32"/>
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="M63">
         <f t="shared" ref="M63:AR63" si="59">M41/M$3</f>
@@ -9054,11 +9054,11 @@
       </c>
       <c r="D64">
         <f t="shared" si="31"/>
-        <v>582</v>
+        <v>522</v>
       </c>
       <c r="E64">
         <f t="shared" si="32"/>
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="M64">
         <f t="shared" ref="M64:AR64" si="60">M42/M$3</f>
@@ -9196,11 +9196,11 @@
       </c>
       <c r="D65">
         <f t="shared" si="31"/>
-        <v>600</v>
+        <v>538</v>
       </c>
       <c r="E65">
         <f t="shared" si="32"/>
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="M65">
         <f t="shared" ref="M65:AR65" si="61">M43/M$3</f>
@@ -9338,11 +9338,11 @@
       </c>
       <c r="D66">
         <f>_xlfn.FLOOR.MATH(LOG(COMBIN($C$32,C66),2))</f>
-        <v>618</v>
+        <v>554</v>
       </c>
       <c r="E66">
         <f t="shared" si="32"/>
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="M66">
         <f t="shared" ref="M66:AR66" si="62">M44/M$3</f>
@@ -9480,11 +9480,11 @@
       </c>
       <c r="D67">
         <f t="shared" ref="D67:D98" si="64">_xlfn.FLOOR.MATH(LOG(COMBIN($C$32,C67),2))</f>
-        <v>636</v>
+        <v>570</v>
       </c>
       <c r="E67">
         <f t="shared" si="32"/>
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="M67">
         <f t="shared" ref="M67:AR67" si="65">M45/M$3</f>
@@ -9622,11 +9622,11 @@
       </c>
       <c r="D68">
         <f t="shared" si="64"/>
-        <v>654</v>
+        <v>586</v>
       </c>
       <c r="E68">
         <f t="shared" si="32"/>
-        <v>93</v>
+        <v>83</v>
       </c>
     </row>
     <row r="69" spans="3:44" x14ac:dyDescent="0.3">
@@ -9636,11 +9636,11 @@
       </c>
       <c r="D69">
         <f t="shared" si="64"/>
-        <v>672</v>
+        <v>602</v>
       </c>
       <c r="E69">
         <f t="shared" si="32"/>
-        <v>96</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="3:44" x14ac:dyDescent="0.3">
@@ -9650,11 +9650,11 @@
       </c>
       <c r="D70">
         <f t="shared" si="64"/>
-        <v>689</v>
+        <v>617</v>
       </c>
       <c r="E70">
         <f t="shared" si="32"/>
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="71" spans="3:44" x14ac:dyDescent="0.3">
@@ -9664,11 +9664,11 @@
       </c>
       <c r="D71">
         <f t="shared" si="64"/>
-        <v>707</v>
+        <v>633</v>
       </c>
       <c r="E71">
         <f t="shared" si="32"/>
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="3:44" x14ac:dyDescent="0.3">
@@ -9678,11 +9678,11 @@
       </c>
       <c r="D72">
         <f t="shared" si="64"/>
-        <v>725</v>
+        <v>649</v>
       </c>
       <c r="E72">
         <f t="shared" si="32"/>
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="73" spans="3:44" x14ac:dyDescent="0.3">
@@ -9692,11 +9692,11 @@
       </c>
       <c r="D73">
         <f t="shared" si="64"/>
-        <v>743</v>
+        <v>665</v>
       </c>
       <c r="E73">
         <f t="shared" si="32"/>
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="74" spans="3:44" x14ac:dyDescent="0.3">
@@ -9706,11 +9706,11 @@
       </c>
       <c r="D74">
         <f t="shared" si="64"/>
-        <v>760</v>
+        <v>680</v>
       </c>
       <c r="E74">
         <f t="shared" si="32"/>
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="75" spans="3:44" x14ac:dyDescent="0.3">
@@ -9720,11 +9720,11 @@
       </c>
       <c r="D75">
         <f t="shared" si="64"/>
-        <v>778</v>
+        <v>696</v>
       </c>
       <c r="E75">
         <f t="shared" si="32"/>
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="76" spans="3:44" x14ac:dyDescent="0.3">
@@ -9734,11 +9734,11 @@
       </c>
       <c r="D76">
         <f t="shared" si="64"/>
-        <v>796</v>
+        <v>712</v>
       </c>
       <c r="E76">
         <f t="shared" si="32"/>
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="77" spans="3:44" x14ac:dyDescent="0.3">
@@ -9748,11 +9748,11 @@
       </c>
       <c r="D77">
         <f t="shared" si="64"/>
-        <v>813</v>
+        <v>727</v>
       </c>
       <c r="E77">
         <f t="shared" si="32"/>
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="78" spans="3:44" x14ac:dyDescent="0.3">
@@ -9762,11 +9762,11 @@
       </c>
       <c r="D78">
         <f t="shared" si="64"/>
-        <v>831</v>
+        <v>743</v>
       </c>
       <c r="E78">
         <f t="shared" si="32"/>
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="79" spans="3:44" x14ac:dyDescent="0.3">
@@ -9776,11 +9776,11 @@
       </c>
       <c r="D79">
         <f t="shared" si="64"/>
-        <v>848</v>
+        <v>758</v>
       </c>
       <c r="E79">
         <f t="shared" si="32"/>
-        <v>121</v>
+        <v>108</v>
       </c>
     </row>
     <row r="80" spans="3:44" x14ac:dyDescent="0.3">
@@ -9790,11 +9790,11 @@
       </c>
       <c r="D80">
         <f t="shared" si="64"/>
-        <v>866</v>
+        <v>774</v>
       </c>
       <c r="E80">
         <f t="shared" si="32"/>
-        <v>123</v>
+        <v>110</v>
       </c>
     </row>
     <row r="81" spans="3:5" x14ac:dyDescent="0.3">
@@ -9804,11 +9804,11 @@
       </c>
       <c r="D81">
         <f t="shared" si="64"/>
-        <v>883</v>
+        <v>789</v>
       </c>
       <c r="E81">
         <f t="shared" si="32"/>
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="82" spans="3:5" x14ac:dyDescent="0.3">
@@ -9818,11 +9818,11 @@
       </c>
       <c r="D82">
         <f t="shared" si="64"/>
-        <v>901</v>
+        <v>805</v>
       </c>
       <c r="E82">
         <f t="shared" si="32"/>
-        <v>128</v>
+        <v>115</v>
       </c>
     </row>
     <row r="83" spans="3:5" x14ac:dyDescent="0.3">
@@ -9832,25 +9832,25 @@
       </c>
       <c r="D83">
         <f>_xlfn.FLOOR.MATH(LOG(COMBIN($C$32,C83),2))</f>
-        <v>918</v>
+        <v>820</v>
       </c>
       <c r="E83">
         <f t="shared" si="32"/>
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="84" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C84">
-        <f t="shared" ref="C84:C98" si="66">C83+1</f>
+        <f t="shared" ref="C84:C92" si="66">C83+1</f>
         <v>50</v>
       </c>
       <c r="D84">
         <f t="shared" si="64"/>
-        <v>935</v>
+        <v>835</v>
       </c>
       <c r="E84">
         <f t="shared" si="32"/>
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="85" spans="3:5" x14ac:dyDescent="0.3">
@@ -9860,11 +9860,11 @@
       </c>
       <c r="D85">
         <f t="shared" si="64"/>
-        <v>953</v>
+        <v>851</v>
       </c>
       <c r="E85">
         <f t="shared" si="32"/>
-        <v>136</v>
+        <v>121</v>
       </c>
     </row>
     <row r="86" spans="3:5" x14ac:dyDescent="0.3">
@@ -9874,11 +9874,11 @@
       </c>
       <c r="D86">
         <f t="shared" si="64"/>
-        <v>970</v>
+        <v>866</v>
       </c>
       <c r="E86">
         <f t="shared" si="32"/>
-        <v>138</v>
+        <v>123</v>
       </c>
     </row>
     <row r="87" spans="3:5" x14ac:dyDescent="0.3">
@@ -9888,11 +9888,11 @@
       </c>
       <c r="D87">
         <f t="shared" si="64"/>
-        <v>987</v>
+        <v>881</v>
       </c>
       <c r="E87">
         <f t="shared" si="32"/>
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="88" spans="3:5" x14ac:dyDescent="0.3">
@@ -9902,11 +9902,11 @@
       </c>
       <c r="D88">
         <f t="shared" si="64"/>
-        <v>1004</v>
+        <v>896</v>
       </c>
       <c r="E88">
         <f t="shared" si="32"/>
-        <v>143</v>
+        <v>128</v>
       </c>
     </row>
     <row r="89" spans="3:5" x14ac:dyDescent="0.3">
@@ -9916,11 +9916,11 @@
       </c>
       <c r="D89">
         <f t="shared" si="64"/>
-        <v>1022</v>
+        <v>912</v>
       </c>
       <c r="E89">
         <f t="shared" si="32"/>
-        <v>146</v>
+        <v>130</v>
       </c>
     </row>
     <row r="90" spans="3:5" x14ac:dyDescent="0.3">
@@ -9928,13 +9928,13 @@
         <f t="shared" si="66"/>
         <v>56</v>
       </c>
-      <c r="D90" t="e">
+      <c r="D90">
         <f t="shared" si="64"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="E90" t="e">
+        <v>927</v>
+      </c>
+      <c r="E90">
         <f t="shared" si="32"/>
-        <v>#NUM!</v>
+        <v>132</v>
       </c>
     </row>
     <row r="91" spans="3:5" x14ac:dyDescent="0.3">
@@ -9942,13 +9942,13 @@
         <f t="shared" si="66"/>
         <v>57</v>
       </c>
-      <c r="D91" t="e">
+      <c r="D91">
         <f t="shared" si="64"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="E91" t="e">
+        <v>942</v>
+      </c>
+      <c r="E91">
         <f t="shared" si="32"/>
-        <v>#NUM!</v>
+        <v>134</v>
       </c>
     </row>
     <row r="92" spans="3:5" x14ac:dyDescent="0.3">
@@ -9956,13 +9956,13 @@
         <f t="shared" si="66"/>
         <v>58</v>
       </c>
-      <c r="D92" t="e">
+      <c r="D92">
         <f t="shared" si="64"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="E92" t="e">
+        <v>957</v>
+      </c>
+      <c r="E92">
         <f t="shared" si="32"/>
-        <v>#NUM!</v>
+        <v>136</v>
       </c>
     </row>
     <row r="93" spans="3:5" x14ac:dyDescent="0.3">
@@ -9970,13 +9970,13 @@
         <f t="shared" ref="C93:C95" si="67">C92+1</f>
         <v>59</v>
       </c>
-      <c r="D93" t="e">
+      <c r="D93">
         <f t="shared" si="64"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="E93" t="e">
+        <v>972</v>
+      </c>
+      <c r="E93">
         <f t="shared" si="32"/>
-        <v>#NUM!</v>
+        <v>138</v>
       </c>
     </row>
     <row r="94" spans="3:5" x14ac:dyDescent="0.3">
@@ -9984,13 +9984,13 @@
         <f t="shared" si="67"/>
         <v>60</v>
       </c>
-      <c r="D94" t="e">
+      <c r="D94">
         <f t="shared" si="64"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="E94" t="e">
+        <v>987</v>
+      </c>
+      <c r="E94">
         <f t="shared" si="32"/>
-        <v>#NUM!</v>
+        <v>141</v>
       </c>
     </row>
     <row r="95" spans="3:5" x14ac:dyDescent="0.3">
@@ -9998,13 +9998,13 @@
         <f t="shared" si="67"/>
         <v>61</v>
       </c>
-      <c r="D95" t="e">
+      <c r="D95">
         <f t="shared" si="64"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="E95" t="e">
+        <v>1002</v>
+      </c>
+      <c r="E95">
         <f t="shared" si="32"/>
-        <v>#NUM!</v>
+        <v>143</v>
       </c>
     </row>
     <row r="96" spans="3:5" x14ac:dyDescent="0.3">
@@ -10012,13 +10012,13 @@
         <f t="shared" ref="C96:C98" si="68">C95+1</f>
         <v>62</v>
       </c>
-      <c r="D96" t="e">
+      <c r="D96">
         <f t="shared" si="64"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="E96" t="e">
+        <v>1017</v>
+      </c>
+      <c r="E96">
         <f t="shared" si="32"/>
-        <v>#NUM!</v>
+        <v>145</v>
       </c>
     </row>
     <row r="97" spans="3:5" x14ac:dyDescent="0.3">

</xml_diff>